<commit_message>
Single player mode AI constructed
</commit_message>
<xml_diff>
--- a/Four-in-a-row- AI logic simul.xlsx
+++ b/Four-in-a-row- AI logic simul.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="99">
   <si>
     <t>['X', 'X', 0, 'P']</t>
   </si>
@@ -923,7 +923,7 @@
   <dimension ref="B1:AP1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1548,15 +1548,15 @@
       </c>
       <c r="AC11" s="20">
         <f t="shared" ref="AC11:AC15" si="2">H13</f>
-        <v>1</v>
-      </c>
-      <c r="AD11" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="20">
         <f t="shared" ref="AD11:AD14" si="3">I14</f>
-        <v>X</v>
-      </c>
-      <c r="AE11" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="20">
         <f t="shared" ref="AE11:AE13" si="4">J15</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AF11" s="19" t="s">
         <v>28</v>
@@ -1569,9 +1569,9 @@
         <f t="shared" ref="AK11:AN11" si="5">IF(AND(AB11=0,AB12=0),IF(AND(AB11=0,AB12=0,AB13=0),"X","P"),AB11)</f>
         <v>X</v>
       </c>
-      <c r="AL11" s="22">
+      <c r="AL11" s="22" t="str">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="AM11" s="22" t="str">
         <f t="shared" si="5"/>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="AO11" s="1" t="str">
         <f t="shared" ref="AO11:AO16" si="6">CONCATENATE(AH11,AI11,AJ11,AK11,AL11,AM11,AN11)</f>
-        <v>X1XX</v>
+        <v>XXXX</v>
       </c>
       <c r="AP11" s="1"/>
     </row>
@@ -1637,11 +1637,11 @@
       </c>
       <c r="R12" s="20">
         <f>MAX(Sheet2!U3:U17)</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="S12" s="20">
         <f>MAX(Sheet2!V3:V17)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T12" s="20">
         <f>MAX(Sheet2!W3:W17)</f>
@@ -1677,15 +1677,15 @@
       </c>
       <c r="AC12" s="20">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD12" s="20">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AE12" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="20">
         <f t="shared" si="4"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AF12" s="19" t="s">
         <v>28</v>
@@ -1699,23 +1699,23 @@
       </c>
       <c r="AK12" s="22" t="str">
         <f t="shared" si="9"/>
-        <v>P</v>
-      </c>
-      <c r="AL12" s="22">
+        <v>X</v>
+      </c>
+      <c r="AL12" s="22" t="str">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AM12" s="22">
+        <v>X</v>
+      </c>
+      <c r="AM12" s="22" t="str">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="AN12" s="24" t="str">
         <f>IF(AND(AE12=0,AE13=0),"P",AE12)</f>
-        <v>X</v>
+        <v>P</v>
       </c>
       <c r="AO12" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>XP11X</v>
+        <v>XXXXP</v>
       </c>
       <c r="AP12" s="1"/>
     </row>
@@ -1736,7 +1736,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="23">
         <v>0</v>
@@ -1746,19 +1746,19 @@
       </c>
       <c r="K13" s="5">
         <f>MAX(Sheet2!H3:H17)</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L13" s="5">
         <f>MAX(Sheet2!H20:H27)</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M13" s="5">
         <f>MAX(Sheet2!H30:H38)</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N13" s="5">
         <f t="shared" si="7"/>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>16</v>
@@ -1808,17 +1808,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AC13" s="20" t="str">
+      <c r="AC13" s="20">
         <f t="shared" si="2"/>
-        <v>X</v>
-      </c>
-      <c r="AD13" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="20">
         <f t="shared" si="3"/>
-        <v>X</v>
-      </c>
-      <c r="AE13" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="20">
         <f t="shared" si="4"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AF13" s="19" t="s">
         <v>28</v>
@@ -1827,15 +1827,15 @@
       <c r="AH13" s="19"/>
       <c r="AI13" s="21" t="str">
         <f t="shared" ref="AI13:AL13" si="11">IF(AND(Z13=0,Z14=0),IF(AND(Z13=0,Z14=0,Z15=0),"X","P"),Z13)</f>
-        <v>P</v>
+        <v>X</v>
       </c>
       <c r="AJ13" s="26" t="str">
         <f t="shared" si="11"/>
-        <v>P</v>
-      </c>
-      <c r="AK13" s="27">
+        <v>X</v>
+      </c>
+      <c r="AK13" s="27" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="AL13" s="27" t="str">
         <f t="shared" si="11"/>
@@ -1843,15 +1843,15 @@
       </c>
       <c r="AM13" s="28" t="str">
         <f>IF(AND(AD13=0,AD14=0),"P",AD13)</f>
-        <v>X</v>
-      </c>
-      <c r="AN13" s="28" t="str">
+        <v>P</v>
+      </c>
+      <c r="AN13" s="28">
         <f>AE13</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AO13" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>PP0XXX</v>
+        <v>XXXXP0</v>
       </c>
       <c r="AP13" s="1"/>
     </row>
@@ -1860,10 +1860,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="23">
         <v>0</v>
@@ -1872,17 +1872,17 @@
         <v>0</v>
       </c>
       <c r="H14" s="25">
-        <v>1</v>
-      </c>
-      <c r="I14" s="25" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="I14" s="25">
+        <v>0</v>
       </c>
       <c r="J14" s="23">
         <v>0</v>
       </c>
       <c r="K14" s="5">
         <f>MAX(Sheet2!G3:G17)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L14" s="5">
         <f>MAX(Sheet2!G20:G27)</f>
@@ -1894,7 +1894,7 @@
       </c>
       <c r="N14" s="5">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>17</v>
@@ -1943,15 +1943,15 @@
       </c>
       <c r="AB14" s="20">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC14" s="20">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD14" s="20">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE14" s="19" t="s">
         <v>28</v>
@@ -1962,32 +1962,32 @@
       <c r="AG14" s="3"/>
       <c r="AH14" s="21" t="str">
         <f t="shared" ref="AH14:AK14" si="13">IF(AND(Y14=0,Y15=0),IF(AND(Y14=0,Y15=0,Y16=0),"X","P"),Y14)</f>
+        <v>X</v>
+      </c>
+      <c r="AI14" s="26" t="str">
+        <f t="shared" si="13"/>
+        <v>X</v>
+      </c>
+      <c r="AJ14" s="27" t="str">
+        <f t="shared" si="13"/>
+        <v>X</v>
+      </c>
+      <c r="AK14" s="27" t="str">
+        <f t="shared" si="13"/>
+        <v>X</v>
+      </c>
+      <c r="AL14" s="28" t="str">
+        <f>IF(AND(AC14=0,AC15=0),"P",AC14)</f>
         <v>P</v>
-      </c>
-      <c r="AI14" s="26">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="27">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AK14" s="27">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="AL14" s="28">
-        <f>IF(AND(AC14=0,AC15=0),"P",AC14)</f>
-        <v>1</v>
       </c>
       <c r="AM14" s="28">
         <f>AD14</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN14" s="19"/>
       <c r="AO14" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>P00111</v>
+        <v>XXXXP0</v>
       </c>
       <c r="AP14" s="1"/>
     </row>
@@ -1996,25 +1996,25 @@
         <v>4</v>
       </c>
       <c r="D15" s="25">
-        <v>1</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="E15" s="25">
+        <v>0</v>
       </c>
       <c r="F15" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="25">
-        <v>1</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="H15" s="25">
+        <v>0</v>
       </c>
       <c r="I15" s="25">
-        <v>1</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="J15" s="25">
+        <v>0</v>
       </c>
       <c r="K15" s="5">
         <f>MAX(Sheet2!F3:F17)</f>
@@ -2041,11 +2041,11 @@
       </c>
       <c r="R15" s="20">
         <f t="shared" si="14"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="S15" s="20">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="T15" s="20">
         <f t="shared" si="14"/>
@@ -2071,19 +2071,19 @@
       </c>
       <c r="Z15" s="20">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA15" s="20">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB15" s="20">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC15" s="20">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD15" s="19" t="s">
         <v>28</v>
@@ -2093,31 +2093,31 @@
       </c>
       <c r="AF15" s="3"/>
       <c r="AG15" s="3"/>
-      <c r="AH15" s="26">
+      <c r="AH15" s="26" t="str">
         <f t="shared" ref="AH15:AJ15" si="15">IF(AND(Y15=0,Y16=0),IF(AND(Y15=0,Y16=0,Y17=0),"X","P"),Y15)</f>
-        <v>0</v>
-      </c>
-      <c r="AI15" s="29">
+        <v>X</v>
+      </c>
+      <c r="AI15" s="29" t="str">
         <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="AJ15" s="27">
+        <v>X</v>
+      </c>
+      <c r="AJ15" s="27" t="str">
         <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="AK15" s="28">
+        <v>X</v>
+      </c>
+      <c r="AK15" s="28" t="str">
         <f>IF(AND(AB15=0,AB16=0),"P",AB15)</f>
-        <v>1</v>
+        <v>P</v>
       </c>
       <c r="AL15" s="28">
         <f>AC15</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM15" s="19"/>
       <c r="AN15" s="19"/>
       <c r="AO15" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>01111</v>
+        <v>XXXP0</v>
       </c>
       <c r="AP15" s="1"/>
     </row>
@@ -2125,26 +2125,26 @@
       <c r="C16" s="15">
         <v>5</v>
       </c>
-      <c r="D16" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>28</v>
+      <c r="D16" s="25">
+        <v>0</v>
+      </c>
+      <c r="E16" s="25">
+        <v>0</v>
       </c>
       <c r="F16" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="25">
-        <v>1</v>
-      </c>
-      <c r="I16" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="I16" s="25">
+        <v>0</v>
+      </c>
+      <c r="J16" s="25">
+        <v>0</v>
       </c>
       <c r="K16" s="5">
         <f>MAX(Sheet2!E3:E17)</f>
@@ -2176,19 +2176,19 @@
       </c>
       <c r="Y16" s="20">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="Z16" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="20">
         <f t="shared" si="10"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AA16" s="20">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB16" s="20">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC16" s="19" t="s">
         <v>28</v>
@@ -2199,28 +2199,28 @@
       <c r="AE16" s="19"/>
       <c r="AF16" s="3"/>
       <c r="AG16" s="3"/>
-      <c r="AH16" s="29">
+      <c r="AH16" s="29" t="str">
         <f t="shared" ref="AH16:AI16" si="16">IF(AND(Y16=0,Y17=0),IF(AND(Y16=0,Y17=0,Y18=0),"X","P"),Y16)</f>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="AI16" s="27" t="str">
         <f t="shared" si="16"/>
         <v>X</v>
       </c>
-      <c r="AJ16" s="28">
+      <c r="AJ16" s="28" t="str">
         <f>IF(AND(AA16=0,AA17=0),"P",AA16)</f>
-        <v>1</v>
+        <v>P</v>
       </c>
       <c r="AK16" s="28">
         <f>AB16</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL16" s="19"/>
       <c r="AM16" s="19"/>
       <c r="AN16" s="19"/>
       <c r="AO16" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>1X11</v>
+        <v>XXP0</v>
       </c>
       <c r="AP16" s="1"/>
     </row>
@@ -2232,22 +2232,22 @@
         <v>28</v>
       </c>
       <c r="E17" s="25">
-        <v>1</v>
-      </c>
-      <c r="F17" s="25" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="F17" s="25">
+        <v>0</v>
       </c>
       <c r="G17" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" s="25">
-        <v>1</v>
-      </c>
-      <c r="J17" s="25" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="J17" s="25">
+        <v>0</v>
       </c>
       <c r="K17" s="5">
         <f>MAX(Sheet2!D3:D17)</f>
@@ -2274,15 +2274,15 @@
       <c r="W17" s="4"/>
       <c r="Y17" s="30">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="Z17" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="30">
         <f t="shared" si="10"/>
-        <v>X</v>
-      </c>
-      <c r="AA17" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="30">
         <f t="shared" si="8"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AB17" s="19"/>
       <c r="AC17" s="3"/>
@@ -2318,13 +2318,13 @@
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
       <c r="W18" s="4"/>
-      <c r="Y18" s="30" t="str">
+      <c r="Y18" s="30">
         <f t="shared" si="12"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="Z18" s="30">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA18" s="19"/>
       <c r="AB18" s="3"/>
@@ -2347,7 +2347,7 @@
       </c>
       <c r="D19" s="5">
         <f>MAX(Sheet2!K3:K17)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E19" s="5">
         <f>MAX(Sheet2!L3:L17)</f>
@@ -2355,11 +2355,11 @@
       </c>
       <c r="F19" s="5">
         <f>MAX(Sheet2!M3:M17)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G19" s="5">
         <f>MAX(Sheet2!N3:N17)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H19" s="5">
         <f>MAX(Sheet2!O3:O17)</f>
@@ -2530,7 +2530,7 @@
       </c>
       <c r="D22" s="5">
         <f t="shared" ref="D22:J22" si="17">SUM(D19:D21)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="17"/>
@@ -2538,11 +2538,11 @@
       </c>
       <c r="F22" s="5">
         <f t="shared" si="17"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G22" s="5">
         <f t="shared" si="17"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H22" s="5">
         <f t="shared" si="17"/>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="N22" s="5">
         <f>SUM(D22:J22,N12:N17,Q15:V15,Q33:V33)</f>
-        <v>1067</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
@@ -3008,7 +3008,7 @@
       </c>
       <c r="Q30" s="20">
         <f>MAX(Sheet2!AB3:AB17)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="R30" s="20">
         <f>MAX(Sheet2!AC3:AC17)</f>
@@ -3016,11 +3016,11 @@
       </c>
       <c r="S30" s="20">
         <f>MAX(Sheet2!AD3:AD17)</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="T30" s="20">
         <f>MAX(Sheet2!AE3:AE17)</f>
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="U30" s="20">
         <f>MAX(Sheet2!AF3:AF17)</f>
@@ -3051,11 +3051,11 @@
       </c>
       <c r="AD30" s="20">
         <f t="shared" ref="AD30:AD33" si="20">E14</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE30" s="20">
         <f t="shared" ref="AE30:AE32" si="21">D15</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF30" s="32" t="s">
         <v>28</v>
@@ -3070,19 +3070,19 @@
       </c>
       <c r="AL30" s="3" t="str">
         <f t="shared" si="22"/>
+        <v>X</v>
+      </c>
+      <c r="AM30" s="3" t="str">
+        <f t="shared" si="22"/>
+        <v>X</v>
+      </c>
+      <c r="AN30" s="3" t="str">
+        <f t="shared" si="22"/>
         <v>P</v>
-      </c>
-      <c r="AM30" s="3">
-        <f t="shared" si="22"/>
-        <v>1</v>
-      </c>
-      <c r="AN30" s="3">
-        <f t="shared" si="22"/>
-        <v>1</v>
       </c>
       <c r="AO30" s="1" t="str">
         <f t="shared" ref="AO30:AO35" si="23">CONCATENATE(AH30,AI30,AJ30,AK30,AL30,AM30,AN30)</f>
-        <v>XP11</v>
+        <v>XXXP</v>
       </c>
       <c r="AP30" s="18" t="s">
         <v>63</v>
@@ -3150,13 +3150,13 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="AD31" s="20" t="str">
+      <c r="AD31" s="20">
         <f t="shared" si="20"/>
-        <v>X</v>
-      </c>
-      <c r="AE31" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="20">
         <f t="shared" si="21"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AF31" s="32" t="s">
         <v>28</v>
@@ -3164,29 +3164,29 @@
       <c r="AG31" s="3"/>
       <c r="AH31" s="19"/>
       <c r="AI31" s="19"/>
-      <c r="AJ31" s="20">
+      <c r="AJ31" s="20" t="str">
         <f t="shared" ref="AJ31:AM31" si="25">IF(AND(AA31=0,AA32=0),IF(AND(AA31=0,AA32=0,AA33=0),"X","P"),AA31)</f>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="AK31" s="20" t="str">
         <f t="shared" si="25"/>
-        <v>P</v>
-      </c>
-      <c r="AL31" s="20">
+        <v>X</v>
+      </c>
+      <c r="AL31" s="20" t="str">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="AM31" s="20" t="str">
         <f t="shared" si="25"/>
         <v>X</v>
       </c>
-      <c r="AN31" s="3" t="str">
+      <c r="AN31" s="3">
         <f>IF(AND(AE31=0,AE32=0),"P",AE31)</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AO31" s="1" t="str">
         <f t="shared" si="23"/>
-        <v>0P0XX</v>
+        <v>XXXX0</v>
       </c>
       <c r="AP31" s="18" t="s">
         <v>69</v>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="AA32" s="20">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB32" s="20">
         <f t="shared" si="18"/>
@@ -3253,11 +3253,11 @@
       </c>
       <c r="AC32" s="20">
         <f t="shared" si="19"/>
-        <v>1</v>
-      </c>
-      <c r="AD32" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="20">
         <f t="shared" si="20"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AE32" s="20" t="str">
         <f t="shared" si="21"/>
@@ -3270,23 +3270,23 @@
       <c r="AH32" s="19"/>
       <c r="AI32" s="3" t="str">
         <f t="shared" ref="AI32:AL32" si="27">IF(AND(Z32=0,Z33=0),IF(AND(Z32=0,Z33=0,Z34=0),"X","P"),Z32)</f>
-        <v>P</v>
-      </c>
-      <c r="AJ32" s="20">
+        <v>X</v>
+      </c>
+      <c r="AJ32" s="20" t="str">
         <f t="shared" si="27"/>
-        <v>1</v>
-      </c>
-      <c r="AK32" s="20">
+        <v>X</v>
+      </c>
+      <c r="AK32" s="20" t="str">
         <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="AL32" s="20">
+        <v>X</v>
+      </c>
+      <c r="AL32" s="20" t="str">
         <f t="shared" si="27"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="AM32" s="20" t="str">
         <f>IF(AND(AD32=0,AD33=0),"P",AD32)</f>
-        <v>X</v>
+        <v>P</v>
       </c>
       <c r="AN32" s="20" t="str">
         <f>AE32</f>
@@ -3294,7 +3294,7 @@
       </c>
       <c r="AO32" s="1" t="str">
         <f t="shared" si="23"/>
-        <v>P101XX</v>
+        <v>XXXXPX</v>
       </c>
       <c r="AP32" s="18" t="s">
         <v>71</v>
@@ -3318,7 +3318,7 @@
       </c>
       <c r="Q33" s="20">
         <f t="shared" ref="Q33:V33" si="28">SUM(Q30:Q32)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="R33" s="20">
         <f t="shared" si="28"/>
@@ -3326,11 +3326,11 @@
       </c>
       <c r="S33" s="20">
         <f t="shared" si="28"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="T33" s="20">
         <f t="shared" si="28"/>
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="U33" s="20">
         <f t="shared" si="28"/>
@@ -3354,19 +3354,19 @@
       </c>
       <c r="AA33" s="20">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB33" s="20">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC33" s="20">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD33" s="20">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE33" s="19" t="s">
         <v>28</v>
@@ -3379,30 +3379,30 @@
         <f t="shared" ref="AH33:AK33" si="30">IF(AND(Y33=0,Y34=0),IF(AND(Y33=0,Y34=0,Y35=0),"X","P"),Y33)</f>
         <v>X</v>
       </c>
-      <c r="AI33" s="3">
+      <c r="AI33" s="3" t="str">
         <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="AJ33" s="20">
+        <v>X</v>
+      </c>
+      <c r="AJ33" s="20" t="str">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="AK33" s="20">
+        <v>X</v>
+      </c>
+      <c r="AK33" s="20" t="str">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="AL33" s="20">
+        <v>X</v>
+      </c>
+      <c r="AL33" s="20" t="str">
         <f>IF(AND(AC33=0,AC34=0),"P",AC33)</f>
-        <v>1</v>
+        <v>P</v>
       </c>
       <c r="AM33" s="20">
         <f>AD33</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN33" s="19"/>
       <c r="AO33" s="1" t="str">
         <f t="shared" si="23"/>
-        <v>X01111</v>
+        <v>XXXXP0</v>
       </c>
       <c r="AP33" s="18" t="s">
         <v>77</v>
@@ -3435,21 +3435,21 @@
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="Z34" s="20" t="str">
+      <c r="Z34" s="20">
         <f t="shared" si="26"/>
-        <v>X</v>
-      </c>
-      <c r="AA34" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="20">
         <f t="shared" si="24"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AB34" s="20">
         <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="AC34" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="20">
         <f t="shared" si="19"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AD34" s="19" t="s">
         <v>28</v>
@@ -3461,7 +3461,7 @@
       <c r="AG34" s="3"/>
       <c r="AH34" s="3" t="str">
         <f t="shared" ref="AH34:AJ34" si="31">IF(AND(Y34=0,Y35=0),IF(AND(Y34=0,Y35=0,Y36=0),"X","P"),Y34)</f>
-        <v>P</v>
+        <v>X</v>
       </c>
       <c r="AI34" s="20" t="str">
         <f t="shared" si="31"/>
@@ -3471,19 +3471,19 @@
         <f t="shared" si="31"/>
         <v>X</v>
       </c>
-      <c r="AK34" s="20">
+      <c r="AK34" s="20" t="str">
         <f>IF(AND(AB34=0,AB35=0),"P",AB34)</f>
-        <v>1</v>
-      </c>
-      <c r="AL34" s="20" t="str">
+        <v>P</v>
+      </c>
+      <c r="AL34" s="20">
         <f>AC34</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AM34" s="19"/>
       <c r="AN34" s="19"/>
       <c r="AO34" s="1" t="str">
         <f t="shared" si="23"/>
-        <v>PXX1X</v>
+        <v>XXXP0</v>
       </c>
       <c r="AP34" s="18" t="s">
         <v>79</v>
@@ -3518,15 +3518,15 @@
       </c>
       <c r="Z35" s="20">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA35" s="20">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB35" s="20">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC35" s="19" t="s">
         <v>28</v>
@@ -3537,28 +3537,28 @@
       <c r="AE35" s="19"/>
       <c r="AF35" s="3"/>
       <c r="AG35" s="3"/>
-      <c r="AH35" s="3">
+      <c r="AH35" s="3" t="str">
         <f t="shared" ref="AH35:AI35" si="32">IF(AND(Y35=0,Y36=0),IF(AND(Y35=0,Y36=0,Y37=0),"X","P"),Y35)</f>
-        <v>0</v>
-      </c>
-      <c r="AI35" s="20">
+        <v>X</v>
+      </c>
+      <c r="AI35" s="20" t="str">
         <f t="shared" si="32"/>
-        <v>1</v>
-      </c>
-      <c r="AJ35" s="20">
+        <v>X</v>
+      </c>
+      <c r="AJ35" s="20" t="str">
         <f>IF(AND(AA35=0,AA36=0),"P",AA35)</f>
-        <v>1</v>
+        <v>P</v>
       </c>
       <c r="AK35" s="20">
         <f>AB35</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL35" s="19"/>
       <c r="AM35" s="19"/>
       <c r="AN35" s="19"/>
       <c r="AO35" s="1" t="str">
         <f t="shared" si="23"/>
-        <v>0111</v>
+        <v>XXP0</v>
       </c>
       <c r="AP35" s="18" t="s">
         <v>81</v>
@@ -3584,17 +3584,17 @@
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
       <c r="W36" s="4"/>
-      <c r="Y36" s="30" t="str">
+      <c r="Y36" s="30">
         <f t="shared" si="29"/>
-        <v>X</v>
-      </c>
-      <c r="Z36" s="30" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="30">
         <f t="shared" si="26"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AA36" s="30">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB36" s="19"/>
       <c r="AC36" s="3"/>
@@ -3633,13 +3633,13 @@
       <c r="U37" s="3"/>
       <c r="V37" s="3"/>
       <c r="W37" s="4"/>
-      <c r="Y37" s="30" t="str">
+      <c r="Y37" s="30">
         <f t="shared" si="29"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="Z37" s="30">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA37" s="19"/>
       <c r="AB37" s="3"/>
@@ -3679,9 +3679,9 @@
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
       <c r="W38" s="4"/>
-      <c r="Y38" s="30" t="str">
+      <c r="Y38" s="30">
         <f t="shared" si="29"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="Z38" s="19"/>
       <c r="AA38" s="3"/>
@@ -3832,11 +3832,11 @@
       </c>
       <c r="AH41" s="3" t="str">
         <f t="shared" ref="AH41:AN41" si="33">IF(AND(D12=0,D13=0),IF(AND(D12=0,D13=0,D14=0),"X","P"),D12)</f>
-        <v>P</v>
+        <v>X</v>
       </c>
       <c r="AI41" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>P</v>
+        <v>X</v>
       </c>
       <c r="AJ41" s="3" t="str">
         <f t="shared" si="33"/>
@@ -3846,13 +3846,13 @@
         <f t="shared" si="33"/>
         <v>X</v>
       </c>
-      <c r="AL41" s="20">
+      <c r="AL41" s="20" t="str">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="AM41" s="3" t="str">
         <f t="shared" si="33"/>
-        <v>P</v>
+        <v>X</v>
       </c>
       <c r="AN41" s="3" t="str">
         <f t="shared" si="33"/>
@@ -3860,7 +3860,7 @@
       </c>
       <c r="AO41" s="1" t="str">
         <f t="shared" ref="AO41:AO46" si="34">CONCATENATE(AH41,AI41,AJ41,AK41,AL41,AM41,AN41)</f>
-        <v>PPXX0PX</v>
+        <v>XXXXXXX</v>
       </c>
       <c r="AP41" s="1"/>
     </row>
@@ -3895,37 +3895,37 @@
       <c r="AG42" s="3">
         <v>2</v>
       </c>
-      <c r="AH42" s="3">
+      <c r="AH42" s="3" t="str">
         <f t="shared" ref="AH42:AN42" si="35">IF(AND(D13=0,D14=0),IF(AND(D13=0,D14=0,D15=0),"X","P"),D13)</f>
-        <v>0</v>
-      </c>
-      <c r="AI42" s="3">
+        <v>X</v>
+      </c>
+      <c r="AI42" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="AJ42" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>P</v>
+        <v>X</v>
       </c>
       <c r="AK42" s="20" t="str">
         <f t="shared" si="35"/>
-        <v>P</v>
-      </c>
-      <c r="AL42" s="20">
+        <v>X</v>
+      </c>
+      <c r="AL42" s="20" t="str">
         <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="AM42" s="3">
+        <v>X</v>
+      </c>
+      <c r="AM42" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="AN42" s="3" t="str">
         <f t="shared" si="35"/>
-        <v>P</v>
+        <v>X</v>
       </c>
       <c r="AO42" s="1" t="str">
         <f t="shared" si="34"/>
-        <v>00PP10P</v>
+        <v>XXXXXXX</v>
       </c>
       <c r="AP42" s="1"/>
     </row>
@@ -3960,37 +3960,37 @@
       <c r="AG43" s="3">
         <v>3</v>
       </c>
-      <c r="AH43" s="3">
+      <c r="AH43" s="3" t="str">
         <f t="shared" ref="AH43:AN43" si="36">IF(AND(D14=0,D15=0),IF(AND(D14=0,D15=0,D16=0),"X","P"),D14)</f>
-        <v>1</v>
-      </c>
-      <c r="AI43" s="3">
+        <v>X</v>
+      </c>
+      <c r="AI43" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>1</v>
-      </c>
-      <c r="AJ43" s="20">
+        <v>X</v>
+      </c>
+      <c r="AJ43" s="20" t="str">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AK43" s="20">
+        <v>X</v>
+      </c>
+      <c r="AK43" s="20" t="str">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AL43" s="20">
+        <v>X</v>
+      </c>
+      <c r="AL43" s="20" t="str">
         <f t="shared" si="36"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="AM43" s="20" t="str">
         <f t="shared" si="36"/>
         <v>X</v>
       </c>
-      <c r="AN43" s="3">
+      <c r="AN43" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>X</v>
       </c>
       <c r="AO43" s="1" t="str">
         <f t="shared" si="34"/>
-        <v>11001X0</v>
+        <v>XXXXXXX</v>
       </c>
       <c r="AP43" s="1"/>
     </row>
@@ -4025,29 +4025,29 @@
       <c r="AG44" s="3">
         <v>4</v>
       </c>
-      <c r="AH44" s="3">
+      <c r="AH44" s="3" t="str">
         <f t="shared" ref="AH44:AN44" si="37">IF(AND(D15=0,D16=0),IF(AND(D15=0,D16=0,D17=0),"X","P"),D15)</f>
-        <v>1</v>
+        <v>P</v>
       </c>
       <c r="AI44" s="20" t="str">
         <f t="shared" si="37"/>
         <v>X</v>
       </c>
-      <c r="AJ44" s="20">
+      <c r="AJ44" s="20" t="str">
         <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
-      <c r="AK44" s="20">
+        <v>X</v>
+      </c>
+      <c r="AK44" s="20" t="str">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="AL44" s="20" t="str">
         <f t="shared" si="37"/>
         <v>X</v>
       </c>
-      <c r="AM44" s="20">
+      <c r="AM44" s="20" t="str">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="AN44" s="3" t="str">
         <f t="shared" si="37"/>
@@ -4055,7 +4055,7 @@
       </c>
       <c r="AO44" s="1" t="str">
         <f t="shared" si="34"/>
-        <v>1X11X1X</v>
+        <v>PXXXXXX</v>
       </c>
       <c r="AP44" s="1"/>
     </row>
@@ -4090,37 +4090,37 @@
       <c r="AG45" s="3">
         <v>5</v>
       </c>
-      <c r="AH45" s="3" t="str">
+      <c r="AH45" s="3">
         <f t="shared" ref="AH45:AN45" si="38">IF(AND(D16=0,D17=0),"P",D16)</f>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AI45" s="20" t="str">
         <f t="shared" si="38"/>
-        <v>X</v>
-      </c>
-      <c r="AJ45" s="20">
+        <v>P</v>
+      </c>
+      <c r="AJ45" s="20" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="AK45" s="20">
+        <v>P</v>
+      </c>
+      <c r="AK45" s="20" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
-      </c>
-      <c r="AL45" s="20">
+        <v>P</v>
+      </c>
+      <c r="AL45" s="20" t="str">
         <f t="shared" si="38"/>
-        <v>1</v>
+        <v>P</v>
       </c>
       <c r="AM45" s="20" t="str">
         <f t="shared" si="38"/>
-        <v>X</v>
+        <v>P</v>
       </c>
       <c r="AN45" s="3" t="str">
         <f t="shared" si="38"/>
-        <v>X</v>
+        <v>P</v>
       </c>
       <c r="AO45" s="1" t="str">
         <f t="shared" si="34"/>
-        <v>XX111XX</v>
+        <v>0PPPPPP</v>
       </c>
       <c r="AP45" s="1"/>
     </row>
@@ -4161,31 +4161,31 @@
       </c>
       <c r="AI46" s="20">
         <f t="shared" si="39"/>
-        <v>1</v>
-      </c>
-      <c r="AJ46" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="AJ46" s="20">
         <f t="shared" si="39"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AK46" s="20">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL46" s="20">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM46" s="20">
         <f t="shared" si="39"/>
-        <v>1</v>
-      </c>
-      <c r="AN46" s="20" t="str">
+        <v>0</v>
+      </c>
+      <c r="AN46" s="20">
         <f t="shared" si="39"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="AO46" s="1" t="str">
         <f t="shared" si="34"/>
-        <v>X1X111X</v>
+        <v>X000000</v>
       </c>
       <c r="AP46" s="1"/>
     </row>
@@ -39540,104 +39540,104 @@
     <row r="1" spans="1:33">
       <c r="D1" s="5" t="str">
         <f>Sheet1!AO46</f>
-        <v>X1X111X</v>
+        <v>X000000</v>
       </c>
       <c r="E1" s="5" t="str">
         <f>Sheet1!AO45</f>
-        <v>XX111XX</v>
+        <v>0PPPPPP</v>
       </c>
       <c r="F1" s="5" t="str">
         <f>Sheet1!AO44</f>
-        <v>1X11X1X</v>
+        <v>PXXXXXX</v>
       </c>
       <c r="G1" s="5" t="str">
         <f>Sheet1!AO43</f>
-        <v>11001X0</v>
+        <v>XXXXXXX</v>
       </c>
       <c r="H1" s="5" t="str">
         <f>Sheet1!AO42</f>
-        <v>00PP10P</v>
+        <v>XXXXXXX</v>
       </c>
       <c r="I1" s="5" t="str">
         <f>Sheet1!AO41</f>
-        <v>PPXX0PX</v>
+        <v>XXXXXXX</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="str">
         <f>CONCATENATE(Sheet1!D12,Sheet1!D13,Sheet1!D14,Sheet1!D15,Sheet1!D16,Sheet1!D17)</f>
-        <v>0011XX</v>
+        <v>00000X</v>
       </c>
       <c r="L1" s="1" t="str">
         <f>CONCATENATE(Sheet1!E12,Sheet1!E13,Sheet1!E14,Sheet1!E15,Sheet1!E16,Sheet1!E17)</f>
-        <v>001XX1</v>
+        <v>000000</v>
       </c>
       <c r="M1" s="1" t="str">
         <f>CONCATENATE(Sheet1!F12,Sheet1!F13,Sheet1!F14,Sheet1!F15,Sheet1!F16,Sheet1!F17)</f>
-        <v>00011X</v>
+        <v>000000</v>
       </c>
       <c r="N1" s="1" t="str">
         <f>CONCATENATE(Sheet1!G12,Sheet1!G13,Sheet1!G14,Sheet1!G15,Sheet1!G16,Sheet1!G17)</f>
-        <v>000111</v>
+        <v>000000</v>
       </c>
       <c r="O1" s="1" t="str">
         <f>CONCATENATE(Sheet1!H12,Sheet1!H13,Sheet1!H14,Sheet1!H15,Sheet1!H16,Sheet1!H17)</f>
-        <v>011X11</v>
+        <v>000000</v>
       </c>
       <c r="P1" s="1" t="str">
         <f>CONCATENATE(Sheet1!I12,Sheet1!I13,Sheet1!I14,Sheet1!I15,Sheet1!I16,Sheet1!I17)</f>
-        <v>00X1X1</v>
+        <v>000000</v>
       </c>
       <c r="Q1" s="1" t="str">
         <f>CONCATENATE(Sheet1!J12,Sheet1!J13,Sheet1!J14,Sheet1!J15,Sheet1!J16,Sheet1!J17)</f>
-        <v>000XXX</v>
+        <v>000000</v>
       </c>
       <c r="T1" s="5" t="str">
         <f>Sheet1!AO16</f>
-        <v>1X11</v>
+        <v>XXP0</v>
       </c>
       <c r="U1" s="5" t="str">
         <f>Sheet1!AO15</f>
-        <v>01111</v>
+        <v>XXXP0</v>
       </c>
       <c r="V1" s="5" t="str">
         <f>Sheet1!AO14</f>
-        <v>P00111</v>
+        <v>XXXXP0</v>
       </c>
       <c r="W1" s="5" t="str">
         <f>Sheet1!AO13</f>
-        <v>PP0XXX</v>
+        <v>XXXXP0</v>
       </c>
       <c r="X1" s="5" t="str">
         <f>Sheet1!AO12</f>
-        <v>XP11X</v>
+        <v>XXXXP</v>
       </c>
       <c r="Y1" s="5" t="str">
         <f>Sheet1!AO11</f>
-        <v>X1XX</v>
+        <v>XXXX</v>
       </c>
       <c r="AB1" s="5" t="str">
         <f>Sheet1!AO35</f>
-        <v>0111</v>
+        <v>XXP0</v>
       </c>
       <c r="AC1" s="5" t="str">
         <f>Sheet1!AO34</f>
-        <v>PXX1X</v>
+        <v>XXXP0</v>
       </c>
       <c r="AD1" s="5" t="str">
         <f>Sheet1!AO33</f>
-        <v>X01111</v>
+        <v>XXXXP0</v>
       </c>
       <c r="AE1" s="5" t="str">
         <f>Sheet1!AO32</f>
-        <v>P101XX</v>
+        <v>XXXXPX</v>
       </c>
       <c r="AF1" s="5" t="str">
         <f>Sheet1!AO31</f>
-        <v>0P0XX</v>
+        <v>XXXX0</v>
       </c>
       <c r="AG1" s="5" t="str">
         <f>Sheet1!AO30</f>
-        <v>XP11</v>
+        <v>XXXP</v>
       </c>
     </row>
     <row r="2" spans="1:33">
@@ -39787,7 +39787,7 @@
       </c>
       <c r="H3" s="1">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" si="0"/>
@@ -39807,11 +39807,11 @@
       </c>
       <c r="M3" s="1">
         <f>IF(ISNUMBER(SEARCH($B3,M$1,1)),$C3,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" s="1">
         <f t="shared" ref="N3:Q17" si="1">IF(ISNUMBER(SEARCH($B3,N$1,1)),$C3,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="1">
         <f t="shared" si="1"/>
@@ -39853,7 +39853,7 @@
   IF(ISNUMBER(SEARCH($B3,V$1,1)),
  $C3,
  0))</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="W3" s="1">
         <f t="shared" si="2"/>
@@ -40076,7 +40076,7 @@
       </c>
       <c r="H5" s="1">
         <f t="shared" si="9"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="9"/>
@@ -40216,7 +40216,7 @@
       </c>
       <c r="H6" s="1">
         <f t="shared" si="13"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="13"/>
@@ -40452,7 +40452,7 @@
       </c>
       <c r="AE7" s="1">
         <f t="shared" si="20"/>
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="AF7" s="1">
         <f t="shared" si="20"/>
@@ -40634,7 +40634,7 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="25"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="25"/>
@@ -40790,7 +40790,7 @@
       </c>
       <c r="K10" s="1">
         <f t="shared" ref="K10:Q10" si="30">IF(ISNUMBER(SEARCH($B10,K$1,1)),$C10,0)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" si="30"/>
@@ -40798,11 +40798,11 @@
       </c>
       <c r="M10" s="1">
         <f t="shared" si="30"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="30"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O10" s="5">
         <f t="shared" si="1"/>
@@ -40835,7 +40835,7 @@
       </c>
       <c r="V10" s="1">
         <f t="shared" si="31"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="W10" s="1">
         <f t="shared" si="31"/>
@@ -40914,7 +40914,7 @@
       </c>
       <c r="G11" s="1">
         <f t="shared" si="33"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="33"/>
@@ -41224,7 +41224,7 @@
       </c>
       <c r="N13" s="1">
         <f t="shared" si="42"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="O13" s="5">
         <f t="shared" si="1"/>
@@ -41253,11 +41253,11 @@
       </c>
       <c r="U13" s="1">
         <f t="shared" si="43"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="V13" s="5">
         <f t="shared" si="43"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="W13" s="1">
         <f t="shared" si="43"/>
@@ -41282,7 +41282,7 @@
   IF(ISNUMBER(SEARCH($B13,AB$1,1)),
  $C13,
  0))</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AC13" s="1">
         <f t="shared" si="44"/>
@@ -41290,7 +41290,7 @@
       </c>
       <c r="AD13" s="1">
         <f t="shared" si="44"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AE13" s="1">
         <f t="shared" si="44"/>
@@ -41815,7 +41815,7 @@
       </c>
       <c r="U17" s="1">
         <f t="shared" si="59"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="V17" s="1">
         <f t="shared" si="59"/>
@@ -41852,7 +41852,7 @@
       </c>
       <c r="AD17" s="1">
         <f t="shared" si="60"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="AE17" s="1">
         <f t="shared" si="60"/>
@@ -41975,7 +41975,7 @@
       </c>
       <c r="H20" s="1">
         <f t="shared" si="62"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="62"/>
@@ -42255,7 +42255,7 @@
       </c>
       <c r="H22" s="1">
         <f t="shared" si="70"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="70"/>
@@ -43172,7 +43172,7 @@
       </c>
       <c r="H30" s="1">
         <f t="shared" si="95"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="I30" s="1">
         <f t="shared" si="95"/>
@@ -43592,7 +43592,7 @@
       </c>
       <c r="H33" s="1">
         <f t="shared" si="107"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I33" s="1">
         <f t="shared" si="107"/>

</xml_diff>